<commit_message>
update yahoo function(dev ing)
</commit_message>
<xml_diff>
--- a/gsout.xlsx
+++ b/gsout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUB-190047\Downloads\IGPWorks\Projects\ASN-GoogleSuggest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUB-190047\Downloads\IGPWorks\Projects\lwrpa-uip-googlesuggest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFD01C8-1FD0-4543-9BB6-15F7F8D87BB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6482C75-5CAF-4547-B41E-ACA44AE8DB59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{68401E15-C423-4926-9280-D03EAC4A0581}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{8894CC8F-C17E-4F09-A507-61C99181D676}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,106 +31,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Keyword</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Suggest</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシー</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシーs9</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシーs10</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシーs8</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシー賞</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシーノート9</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ギャラクシーa30</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ギャラクシー原宿</t>
+  </si>
+  <si>
+    <t>ギャラクシーノート8</t>
   </si>
   <si>
     <t>ギャラクシーs10 カバー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ギャラクシーノート8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ギャラクシーノート</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ギャラクシー </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ギャラクシー 原宿</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>RPA</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa meaning</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa uipath</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa holdings</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpay</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa tools</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa bank</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa digital world 2019</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa ai</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rpa software</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -493,8 +429,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF481439-32A4-46DF-AE98-0B9912C8553B}">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CC5007-CE6A-4028-8E2E-A15480A1CC96}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -588,166 +524,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>